<commit_message>
test success for 4 cases
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22365" windowHeight="12675"/>
+    <workbookView windowWidth="27795" windowHeight="13080"/>
   </bookViews>
   <sheets>
     <sheet name="local from global" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>local_from_global</t>
   </si>
@@ -30,24 +30,58 @@
   <si>
     <t>x_bar</t>
   </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>theta1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>theta2</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Droid Sans Mono"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -58,44 +92,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -110,22 +107,23 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -140,8 +138,15 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,14 +154,29 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,7 +199,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,7 +214,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,7 +237,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,73 +399,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,97 +411,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,11 +440,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -441,7 +483,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -456,36 +513,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -506,154 +533,160 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2620,14 +2653,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>635</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>151130</xdr:rowOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>692150</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>183515</xdr:rowOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>153670</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2635,8 +2668,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="635" y="12305030"/>
-        <a:ext cx="13550265" cy="11138535"/>
+        <a:off x="635" y="14789150"/>
+        <a:ext cx="15045690" cy="11139170"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2936,14 +2969,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
+    <col min="4" max="4" width="13.2"/>
+    <col min="5" max="6" width="12.1333333333333"/>
     <col min="13" max="16" width="9.06666666666667"/>
   </cols>
   <sheetData>
@@ -4719,6 +4754,315 @@
       </c>
       <c r="P41">
         <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1">
+        <v>53.3254760353654</v>
+      </c>
+      <c r="B47" s="1">
+        <v>140.048759360422</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ref="D47:D57" si="0">A47+G47*COS(F47)</f>
+        <v>50.9497021750014</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ref="E47:E57" si="1">B47+G47*SIN(F47)</f>
+        <v>142.618914718452</v>
+      </c>
+      <c r="F47">
+        <f t="shared" ref="F47:F57" si="2">C47+PI()/2</f>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G47">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1">
+        <v>93.7136316615536</v>
+      </c>
+      <c r="B48" s="1">
+        <v>177.382348594713</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>91.3378578011896</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>179.952503952743</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="2"/>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G48">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1">
+        <v>83.4330102294329</v>
+      </c>
+      <c r="B49" s="1">
+        <v>167.879253153257</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>81.0572363690689</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>170.449408511287</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="2"/>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G49">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1">
+        <v>103.994253093674</v>
+      </c>
+      <c r="B50" s="1">
+        <v>186.885444036169</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>101.61847923331</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>189.455599394199</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="2"/>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G50">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1">
+        <v>63.606097467486</v>
+      </c>
+      <c r="B51" s="1">
+        <v>149.551854801878</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>61.230323607122</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>152.122010159908</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="2"/>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G51">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1">
+        <v>58.4657867514257</v>
+      </c>
+      <c r="B52" s="1">
+        <v>144.80030708115</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>56.0900128910617</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>147.37046243918</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="2"/>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G52">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1">
+        <v>125.28982606021</v>
+      </c>
+      <c r="B53" s="1">
+        <v>206.570427450614</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>122.914052199846</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>209.140582808644</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="2"/>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G53">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="1">
+        <v>143.648078617568</v>
+      </c>
+      <c r="B54" s="1">
+        <v>223.540240738928</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>141.272304757204</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="1"/>
+        <v>226.110396096958</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="2"/>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G54">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="2">
+        <v>112.806</v>
+      </c>
+      <c r="B55" s="2">
+        <v>195.031</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>113.00963775946</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>194.810700969312</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="2"/>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G55">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56">
+        <v>33.5</v>
+      </c>
+      <c r="B56">
+        <v>121.72</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>31.124226139636</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="1"/>
+        <v>124.29015535803</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="2"/>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G56">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57">
+        <v>100</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.746117069464104</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>7.62422613963599</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>102.57015535803</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="2"/>
+        <v>2.316913396259</v>
+      </c>
+      <c r="G57">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>